<commit_message>
modification base de datos
Se modifico base de datos agregando nuevos campos.
Se modifico archivo excel.
Se inicio la creación de inserts en archivo excel.
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/database/inserts.xlsx
+++ b/src/main/webapp/WEB-INF/database/inserts.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="32540" windowHeight="20540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="01_seguridad" sheetId="2" r:id="rId1"/>
     <sheet name="02_catalogos" sheetId="1" r:id="rId2"/>
     <sheet name="03_socio" sheetId="3" r:id="rId3"/>
     <sheet name="04_fedaamac" sheetId="4" r:id="rId4"/>
+    <sheet name="05_otros" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="315">
   <si>
     <t>usuario</t>
   </si>
@@ -188,18 +189,12 @@
     <t>'Transferencia entre cuentas'</t>
   </si>
   <si>
-    <t>'Administración'</t>
-  </si>
-  <si>
     <t>'Cuenta de ahorro'</t>
   </si>
   <si>
     <t>'Cuenta de préstamo otorgado'</t>
   </si>
   <si>
-    <t>'Cuenta para administración'</t>
-  </si>
-  <si>
     <t>'BECA EN CHEQUE'</t>
   </si>
   <si>
@@ -740,9 +735,6 @@
     <t>id_clave_movimiento_contable</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>socio_responsable_primero</t>
   </si>
   <si>
@@ -800,9 +792,6 @@
     <t>codigo_postal</t>
   </si>
   <si>
-    <t>paos</t>
-  </si>
-  <si>
     <t>telefono_particular</t>
   </si>
   <si>
@@ -845,9 +834,6 @@
     <t>fecha_vencimiento</t>
   </si>
   <si>
-    <t>reutilizable_cuenta</t>
-  </si>
-  <si>
     <t>movimientos_bancarios</t>
   </si>
   <si>
@@ -867,6 +853,126 @@
   </si>
   <si>
     <t>id_movimiento_bancario</t>
+  </si>
+  <si>
+    <t>reutilizable_clave</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>'Contable'</t>
+  </si>
+  <si>
+    <t>cuentas_bancarias</t>
+  </si>
+  <si>
+    <t>frases_celebres</t>
+  </si>
+  <si>
+    <t>parametros_configuracion</t>
+  </si>
+  <si>
+    <t>id_frase_celebre</t>
+  </si>
+  <si>
+    <t>enunciado</t>
+  </si>
+  <si>
+    <t>autor</t>
+  </si>
+  <si>
+    <t>id_parametro_configuracion</t>
+  </si>
+  <si>
+    <t>valor_int</t>
+  </si>
+  <si>
+    <t>valor_float</t>
+  </si>
+  <si>
+    <t>valor_string</t>
+  </si>
+  <si>
+    <t>valor_boolean</t>
+  </si>
+  <si>
+    <t>'La excelencia es una aspiración humana; la perfección es asunto de Dios'</t>
+  </si>
+  <si>
+    <t>'El dinero no da la felicidad, pero si calma los nervios'</t>
+  </si>
+  <si>
+    <t>'Un buen padre lo es por su corazón y sus entrañas, no por su cerebro'</t>
+  </si>
+  <si>
+    <t>'La felicidad se obtiene dando felicidad'</t>
+  </si>
+  <si>
+    <t>'El dinero no es bueno ni malo, su valor depende de quien lo gana y quien lo gasta'</t>
+  </si>
+  <si>
+    <t>'La ambición sin conocimientos es como un barco fuera del agua'</t>
+  </si>
+  <si>
+    <t>clave_socio</t>
+  </si>
+  <si>
+    <t>'Luis'</t>
+  </si>
+  <si>
+    <t>'López'</t>
+  </si>
+  <si>
+    <t>'Baeza'</t>
+  </si>
+  <si>
+    <t>'David'</t>
+  </si>
+  <si>
+    <t>'Aurora'</t>
+  </si>
+  <si>
+    <t>'María de Jesús'</t>
+  </si>
+  <si>
+    <t>'Yolanda'</t>
+  </si>
+  <si>
+    <t>otro_nombre</t>
+  </si>
+  <si>
+    <t>'María Bertha'</t>
+  </si>
+  <si>
+    <t>'Antonia'</t>
+  </si>
+  <si>
+    <t>'Fernando'</t>
+  </si>
+  <si>
+    <t>'Raúl'</t>
+  </si>
+  <si>
+    <t>'Rosa María'</t>
+  </si>
+  <si>
+    <t>'Diversos no identificados'</t>
+  </si>
+  <si>
+    <t>'Seguro'</t>
+  </si>
+  <si>
+    <t>'Cuenta de seguro por grupo'</t>
+  </si>
+  <si>
+    <t>'Para administración interna del sistema'</t>
+  </si>
+  <si>
+    <t>cuentas_multiples_socios</t>
+  </si>
+  <si>
+    <t>id_cuenta_multiple_socio</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1305,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
@@ -1218,7 +1324,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -1237,7 +1343,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -1261,17 +1367,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I109"/>
+  <dimension ref="B2:I110"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
@@ -1281,18 +1387,18 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" t="s">
         <v>164</v>
-      </c>
-      <c r="C3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" t="s">
-        <v>166</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1306,13 +1412,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1323,13 +1429,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1340,13 +1446,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -1357,13 +1463,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -1374,13 +1480,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1391,13 +1497,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1408,13 +1514,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -1425,13 +1531,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -1442,13 +1548,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -1459,13 +1565,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -1476,13 +1582,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -1493,13 +1599,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -1510,13 +1616,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -1527,13 +1633,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -1544,13 +1650,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -1566,7 +1672,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
@@ -1631,7 +1737,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -1653,10 +1759,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>277</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>56</v>
+        <v>312</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -1667,10 +1773,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>310</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>54</v>
+        <v>311</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -1681,66 +1787,63 @@
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>231</v>
+      <c r="D33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>234</v>
-      </c>
-      <c r="C36" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C37" t="s">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -1748,16 +1851,16 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -1765,72 +1868,72 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41">
         <v>4</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F40" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>232</v>
+      <c r="F41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>235</v>
-      </c>
-      <c r="C44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>233</v>
+      </c>
+      <c r="C45" t="s">
         <v>4</v>
       </c>
-      <c r="D44" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -1838,16 +1941,16 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -1855,16 +1958,16 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -1872,16 +1975,16 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -1889,81 +1992,72 @@
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51">
         <v>6</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>233</v>
+      <c r="F51" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>236</v>
-      </c>
-      <c r="C54" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" t="s">
         <v>42</v>
       </c>
-      <c r="D54" t="s">
-        <v>234</v>
-      </c>
-      <c r="E54" t="s">
-        <v>235</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="D55" t="s">
+        <v>232</v>
+      </c>
+      <c r="E55" t="s">
+        <v>233</v>
+      </c>
+      <c r="F55" t="s">
         <v>4</v>
       </c>
-      <c r="G54" t="s">
-        <v>1</v>
-      </c>
-      <c r="H54" t="s">
-        <v>2</v>
-      </c>
-      <c r="I54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-      <c r="E55">
-        <v>5</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I55" t="b">
-        <v>1</v>
+      <c r="G55" t="s">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1972,16 +2066,16 @@
         <v>2</v>
       </c>
       <c r="E56">
-        <v>3</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>88</v>
+        <v>5</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I56" t="b">
         <v>1</v>
@@ -1989,7 +2083,7 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1998,16 +2092,16 @@
         <v>2</v>
       </c>
       <c r="E57">
-        <v>5</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>89</v>
+        <v>3</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I57" t="b">
         <v>1</v>
@@ -2015,7 +2109,7 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2027,13 +2121,13 @@
         <v>5</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I58" t="b">
         <v>1</v>
@@ -2041,25 +2135,25 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
         <v>5</v>
       </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59">
-        <v>3</v>
-      </c>
       <c r="F59" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I59" t="b">
         <v>1</v>
@@ -2067,7 +2161,7 @@
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2079,13 +2173,13 @@
         <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I60" t="b">
         <v>1</v>
@@ -2093,7 +2187,7 @@
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2105,13 +2199,13 @@
         <v>3</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I61" t="b">
         <v>1</v>
@@ -2119,7 +2213,7 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2128,16 +2222,16 @@
         <v>2</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I62" t="b">
         <v>1</v>
@@ -2145,7 +2239,7 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2157,13 +2251,13 @@
         <v>5</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I63" t="b">
         <v>1</v>
@@ -2171,64 +2265,64 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64">
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65">
         <v>10</v>
       </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64">
-        <v>3</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B66">
-        <v>11</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I66" t="b">
-        <v>1</v>
-      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -2237,16 +2331,16 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="I67" t="b">
         <v>1</v>
@@ -2254,7 +2348,7 @@
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C68">
         <v>2</v>
@@ -2266,13 +2360,13 @@
         <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I68" t="b">
         <v>1</v>
@@ -2280,7 +2374,7 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C69">
         <v>2</v>
@@ -2292,13 +2386,13 @@
         <v>3</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I69" t="b">
         <v>1</v>
@@ -2306,7 +2400,7 @@
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -2315,16 +2409,16 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I70" t="b">
         <v>1</v>
@@ -2332,7 +2426,7 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C71">
         <v>2</v>
@@ -2344,13 +2438,13 @@
         <v>5</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I71" t="b">
         <v>1</v>
@@ -2358,7 +2452,7 @@
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -2370,13 +2464,13 @@
         <v>5</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I72" t="b">
         <v>1</v>
@@ -2384,7 +2478,7 @@
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -2396,13 +2490,13 @@
         <v>5</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I73" t="b">
         <v>1</v>
@@ -2410,7 +2504,7 @@
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -2422,52 +2516,52 @@
         <v>5</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>159</v>
+        <v>102</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="I74" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
+      <c r="B75">
+        <v>19</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>5</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B76">
-        <v>20</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="D76">
-        <v>2</v>
-      </c>
-      <c r="E76">
-        <v>3</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I76" t="b">
-        <v>1</v>
-      </c>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -2479,13 +2573,13 @@
         <v>3</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I77" t="b">
         <v>1</v>
@@ -2493,7 +2587,7 @@
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C78">
         <v>2</v>
@@ -2505,13 +2599,13 @@
         <v>3</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I78" t="b">
         <v>1</v>
@@ -2519,7 +2613,7 @@
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79">
         <v>2</v>
@@ -2528,16 +2622,16 @@
         <v>2</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="I79" t="b">
         <v>1</v>
@@ -2545,7 +2639,7 @@
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C80">
         <v>2</v>
@@ -2557,47 +2651,47 @@
         <v>5</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G80" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>24</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="H81" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I80" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B82">
-        <v>25</v>
-      </c>
-      <c r="C82">
-        <v>3</v>
-      </c>
-      <c r="D82">
-        <v>3</v>
-      </c>
-      <c r="E82">
-        <v>3</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I82" t="b">
+      <c r="I81" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -2606,16 +2700,16 @@
         <v>3</v>
       </c>
       <c r="E83">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="I83" t="b">
         <v>1</v>
@@ -2623,7 +2717,7 @@
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2635,13 +2729,13 @@
         <v>5</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I84" t="b">
         <v>1</v>
@@ -2649,7 +2743,7 @@
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -2658,16 +2752,16 @@
         <v>3</v>
       </c>
       <c r="E85">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>141</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I85" t="b">
         <v>1</v>
@@ -2675,7 +2769,7 @@
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -2684,16 +2778,16 @@
         <v>3</v>
       </c>
       <c r="E86">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="I86" t="b">
         <v>1</v>
@@ -2701,7 +2795,7 @@
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -2710,16 +2804,16 @@
         <v>3</v>
       </c>
       <c r="E87">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I87" t="b">
         <v>1</v>
@@ -2727,7 +2821,7 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -2736,16 +2830,16 @@
         <v>3</v>
       </c>
       <c r="E88">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="I88" t="b">
         <v>1</v>
@@ -2753,64 +2847,64 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89">
+        <v>31</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B90">
         <v>32</v>
       </c>
-      <c r="C89">
-        <v>3</v>
-      </c>
-      <c r="D89">
-        <v>3</v>
-      </c>
-      <c r="E89">
-        <v>3</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I89" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+      <c r="E90">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B91">
-        <v>33</v>
-      </c>
-      <c r="C91">
-        <v>3</v>
-      </c>
-      <c r="D91">
-        <v>4</v>
-      </c>
-      <c r="E91">
-        <v>3</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I91" t="b">
-        <v>1</v>
-      </c>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -2822,13 +2916,13 @@
         <v>3</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I92" t="b">
         <v>1</v>
@@ -2836,7 +2930,7 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C93">
         <v>3</v>
@@ -2848,13 +2942,13 @@
         <v>3</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I93" t="b">
         <v>1</v>
@@ -2862,7 +2956,7 @@
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C94">
         <v>3</v>
@@ -2871,16 +2965,16 @@
         <v>4</v>
       </c>
       <c r="E94">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I94" t="b">
         <v>1</v>
@@ -2888,7 +2982,7 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C95">
         <v>3</v>
@@ -2897,16 +2991,16 @@
         <v>4</v>
       </c>
       <c r="E95">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I95" t="b">
         <v>1</v>
@@ -2914,7 +3008,7 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C96">
         <v>3</v>
@@ -2926,13 +3020,13 @@
         <v>3</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I96" t="b">
         <v>1</v>
@@ -2940,7 +3034,7 @@
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C97">
         <v>3</v>
@@ -2949,16 +3043,16 @@
         <v>4</v>
       </c>
       <c r="E97">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I97" t="b">
         <v>1</v>
@@ -2966,7 +3060,7 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C98">
         <v>3</v>
@@ -2975,25 +3069,46 @@
         <v>4</v>
       </c>
       <c r="E98">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I98" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
+      <c r="B99">
+        <v>40</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99">
+        <v>4</v>
+      </c>
+      <c r="E99">
+        <v>3</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I99" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F100" s="1"/>
@@ -3001,167 +3116,193 @@
       <c r="H100" s="1"/>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>237</v>
-      </c>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>162</v>
-      </c>
-      <c r="C102" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>160</v>
+      </c>
+      <c r="C103" t="s">
         <v>9</v>
       </c>
-      <c r="D102" t="s">
-        <v>238</v>
-      </c>
-      <c r="E102" t="s">
-        <v>239</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="D103" t="s">
+        <v>235</v>
+      </c>
+      <c r="E103" t="s">
+        <v>236</v>
+      </c>
+      <c r="F103" t="s">
         <v>10</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G103" t="s">
         <v>11</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H103" t="s">
         <v>12</v>
       </c>
-      <c r="I102" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C103" s="1" t="s">
+      <c r="I103" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>3</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>4</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>5</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>6</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F103" s="1" t="s">
+      <c r="D109" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G103" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="I103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C104" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F104" s="1" t="s">
+      <c r="H109" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G104" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="I104" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C105" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I105" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C106" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D106" s="1" t="s">
+      <c r="I109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>7</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="I106" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C107" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G107" s="1" t="s">
+      <c r="F110" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="H110" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I107" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C108" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H108" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="I108" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C109" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I109" t="b">
+      <c r="I110" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3173,251 +3314,487 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O11"/>
+  <dimension ref="B2:O25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I3" t="s">
+        <v>303</v>
+      </c>
+      <c r="J3" t="s">
         <v>243</v>
       </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
         <v>244</v>
       </c>
-      <c r="F3" t="s">
+      <c r="L3" t="s">
         <v>245</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>246</v>
       </c>
-      <c r="H3" t="s">
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
         <v>247</v>
       </c>
-      <c r="I3" t="s">
+      <c r="D21" t="s">
         <v>248</v>
       </c>
-      <c r="J3" t="s">
+      <c r="E21" t="s">
         <v>249</v>
       </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F21" t="s">
         <v>250</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G21" t="s">
         <v>251</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H21" t="s">
         <v>252</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I21" t="s">
         <v>253</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J21" t="s">
+        <v>276</v>
+      </c>
+      <c r="K21" t="s">
         <v>254</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L21" t="s">
         <v>255</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M21" t="s">
         <v>256</v>
       </c>
-      <c r="J7" t="s">
+      <c r="N21" t="s">
+        <v>245</v>
+      </c>
+      <c r="O21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>257</v>
       </c>
-      <c r="K7" t="s">
-        <v>258</v>
-      </c>
-      <c r="L7" t="s">
-        <v>259</v>
-      </c>
-      <c r="M7" t="s">
-        <v>260</v>
-      </c>
-      <c r="N7" t="s">
-        <v>248</v>
-      </c>
-      <c r="O7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C11" t="s">
-        <v>243</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E25" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F25" t="s">
         <v>12</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G25" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K27"/>
+  <dimension ref="B2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G3" t="s">
         <v>262</v>
       </c>
-      <c r="C3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
         <v>263</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>264</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F10" t="s">
         <v>265</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>266</v>
       </c>
-      <c r="H3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I10" t="s">
         <v>267</v>
       </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>243</v>
-      </c>
-      <c r="D10" t="s">
-        <v>262</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>269</v>
-      </c>
-      <c r="G10" t="s">
-        <v>270</v>
-      </c>
-      <c r="H10" t="s">
-        <v>271</v>
-      </c>
-      <c r="I10" t="s">
-        <v>272</v>
-      </c>
       <c r="J10" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="K10" t="s">
+        <v>263</v>
+      </c>
+      <c r="L10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C18" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D18" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="G18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H18" t="s">
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="J18" t="s">
         <v>3</v>
@@ -3425,36 +3802,163 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E27" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F27" t="s">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H27" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>314</v>
+      </c>
+      <c r="C34" t="s">
+        <v>272</v>
+      </c>
+      <c r="D34" t="s">
+        <v>240</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B15:H30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>281</v>
+      </c>
+      <c r="C16" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" t="s">
+        <v>283</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>284</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>285</v>
+      </c>
+      <c r="E30" t="s">
+        <v>286</v>
+      </c>
+      <c r="F30" t="s">
+        <v>287</v>
+      </c>
+      <c r="G30" t="s">
+        <v>288</v>
+      </c>
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>